<commit_message>
working customer profile view
</commit_message>
<xml_diff>
--- a/field_mappings.xlsx
+++ b/field_mappings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34440" yWindow="-8220" windowWidth="45380" windowHeight="26260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">    _setup_field(_basic, 0, "profile_image", "Profile Image", _string)</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Indicates liklihood of Being a Charitable Donor", _bool)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    _setup_field(_basic, 1, "social__facebook", "Facebook", _string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    _setup_field(_basic, 1, "social__googleplus", "Google Plus", _string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    _setup_field(_basic, 1, "social__twitter", "Twitter", _string)</t>
   </si>
 </sst>
 </file>
@@ -238,9 +247,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,7 +322,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -313,6 +344,17 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -334,6 +376,17 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -664,25 +717,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I47"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="127" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" customWidth="1"/>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
     <col min="7" max="7" width="69.5" customWidth="1"/>
     <col min="8" max="8" width="75.6640625" customWidth="1"/>
+    <col min="9" max="9" width="126.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,1706 +772,2017 @@
         <f>SUBSTITUTE(A1,D1,CONCATENATE("CUSTOMER_FIELD_NAMES.",E1))</f>
         <v xml:space="preserve">    _setup_field(_basic, 0, CUSTOMER_FIELD_NAMES.profile_image, "Profile Image", _string)</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="K1" t="str">
+        <f>CONCATENATE("def get_",E1,"(self):")</f>
+        <v>def get_profile_image(self):</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B47" si="0">RIGHT(A2, LEN(A2)-FIND("""",A2))</f>
-        <v>first_name", "First Name", _string)</v>
+        <f>RIGHT(A2, LEN(A2)-FIND("""",A2))</f>
+        <v>social__facebook", "Facebook", _string)</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C47" si="1">LEFT(RIGHT(A2, LEN(A2)-FIND("""",A2)), FIND("""",B2)-1)</f>
-        <v>first_name</v>
+        <f>LEFT(RIGHT(A2, LEN(A2)-FIND("""",A2)), FIND("""",B2)-1)</f>
+        <v>social__facebook</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D47" si="2">CONCATENATE("""",C2,"""")</f>
-        <v>"first_name"</v>
+        <f>CONCATENATE("""",C2,"""")</f>
+        <v>"social__facebook"</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f t="shared" ref="E2:E47" si="3">SUBSTITUTE(C2, "#","__")</f>
-        <v>first_name</v>
+        <f>SUBSTITUTE(C2, "#","__")</f>
+        <v>social__facebook</v>
       </c>
       <c r="F2" t="str">
         <f>RIGHT(B2, LEN(B2)-FIND("""",B2)-3)</f>
-        <v>First Name", _string)</v>
+        <v>Facebook", _string)</v>
       </c>
       <c r="G2" s="2" t="str">
-        <f t="shared" ref="G2:G47" si="4">LEFT(F2,FIND("""",F2)-1)</f>
-        <v>First Name</v>
+        <f>LEFT(F2,FIND("""",F2)-1)</f>
+        <v>Facebook</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H47" si="5">CONCATENATE("('",E2,"', '",G2,"'),")</f>
-        <v>('first_name', 'First Name'),</v>
+        <f>CONCATENATE("('",E2,"', '",G2,"'),")</f>
+        <v>('social__facebook', 'Facebook'),</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I47" si="6">SUBSTITUTE(A2,D2,CONCATENATE("CUSTOMER_FIELD_NAMES.",E2))</f>
-        <v xml:space="preserve">    _setup_field(_basic, 100, CUSTOMER_FIELD_NAMES.first_name, "First Name", _string)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>2</v>
+        <f>SUBSTITUTE(A2,D2,CONCATENATE("CUSTOMER_FIELD_NAMES.",E2))</f>
+        <v xml:space="preserve">    _setup_field(_basic, 1, CUSTOMER_FIELD_NAMES.social__facebook, "Facebook", _string)</v>
+      </c>
+      <c r="K2" t="str">
+        <f>CONCATENATE("def get_",E2,"(self):")</f>
+        <v>def get_social__facebook(self):</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>last_name", "Last Name", _string)</v>
+        <f>RIGHT(A3, LEN(A3)-FIND("""",A3))</f>
+        <v>social__twitter", "Twitter", _string)</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="1"/>
-        <v>last_name</v>
+        <f>LEFT(RIGHT(A3, LEN(A3)-FIND("""",A3)), FIND("""",B3)-1)</f>
+        <v>social__twitter</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="2"/>
-        <v>"last_name"</v>
+        <f>CONCATENATE("""",C3,"""")</f>
+        <v>"social__twitter"</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>last_name</v>
+        <f>SUBSTITUTE(C3, "#","__")</f>
+        <v>social__twitter</v>
       </c>
       <c r="F3" t="str">
         <f>RIGHT(B3, LEN(B3)-FIND("""",B3)-3)</f>
-        <v>Last Name", _string)</v>
+        <v>Twitter", _string)</v>
       </c>
       <c r="G3" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Last Name</v>
+        <f>LEFT(F3,FIND("""",F3)-1)</f>
+        <v>Twitter</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" si="5"/>
-        <v>('last_name', 'Last Name'),</v>
+        <f>CONCATENATE("('",E3,"', '",G3,"'),")</f>
+        <v>('social__twitter', 'Twitter'),</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 200, CUSTOMER_FIELD_NAMES.last_name, "Last Name", _string)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>3</v>
+        <f>SUBSTITUTE(A3,D3,CONCATENATE("CUSTOMER_FIELD_NAMES.",E3))</f>
+        <v xml:space="preserve">    _setup_field(_basic, 1, CUSTOMER_FIELD_NAMES.social__twitter, "Twitter", _string)</v>
+      </c>
+      <c r="K3" t="str">
+        <f>CONCATENATE("def get_",E3,"(self):")</f>
+        <v>def get_social__twitter(self):</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>dob", "Birthday", _date)</v>
+        <f>RIGHT(A4, LEN(A4)-FIND("""",A4))</f>
+        <v>social__googleplus", "Google Plus", _string)</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v>dob</v>
+        <f>LEFT(RIGHT(A4, LEN(A4)-FIND("""",A4)), FIND("""",B4)-1)</f>
+        <v>social__googleplus</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="2"/>
-        <v>"dob"</v>
+        <f>CONCATENATE("""",C4,"""")</f>
+        <v>"social__googleplus"</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>dob</v>
+        <f>SUBSTITUTE(C4, "#","__")</f>
+        <v>social__googleplus</v>
       </c>
       <c r="F4" t="str">
         <f>RIGHT(B4, LEN(B4)-FIND("""",B4)-3)</f>
-        <v>Birthday", _date)</v>
+        <v>Google Plus", _string)</v>
       </c>
       <c r="G4" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Birthday</v>
+        <f>LEFT(F4,FIND("""",F4)-1)</f>
+        <v>Google Plus</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="5"/>
-        <v>('dob', 'Birthday'),</v>
+        <f>CONCATENATE("('",E4,"', '",G4,"'),")</f>
+        <v>('social__googleplus', 'Google Plus'),</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 300, CUSTOMER_FIELD_NAMES.dob, "Birthday", _date)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <f>SUBSTITUTE(A4,D4,CONCATENATE("CUSTOMER_FIELD_NAMES.",E4))</f>
+        <v xml:space="preserve">    _setup_field(_basic, 1, CUSTOMER_FIELD_NAMES.social__googleplus, "Google Plus", _string)</v>
+      </c>
+      <c r="K4" t="str">
+        <f>CONCATENATE("def get_",E4,"(self):")</f>
+        <v>def get_social__googleplus(self):</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>age", "Age", _string)</v>
+        <f t="shared" ref="B5:B50" si="0">RIGHT(A5, LEN(A5)-FIND("""",A5))</f>
+        <v>first_name", "First Name", _string)</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>age</v>
+        <f t="shared" ref="C5:C50" si="1">LEFT(RIGHT(A5, LEN(A5)-FIND("""",A5)), FIND("""",B5)-1)</f>
+        <v>first_name</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>"age"</v>
+        <f t="shared" ref="D5:D50" si="2">CONCATENATE("""",C5,"""")</f>
+        <v>"first_name"</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>age</v>
+        <f t="shared" ref="E5:E50" si="3">SUBSTITUTE(C5, "#","__")</f>
+        <v>first_name</v>
       </c>
       <c r="F5" t="str">
         <f>RIGHT(B5, LEN(B5)-FIND("""",B5)-3)</f>
-        <v>Age", _string)</v>
+        <v>First Name", _string)</v>
       </c>
       <c r="G5" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Age</v>
+        <f t="shared" ref="G5:G50" si="4">LEFT(F5,FIND("""",F5)-1)</f>
+        <v>First Name</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="5"/>
-        <v>('age', 'Age'),</v>
+        <f t="shared" ref="H5:H50" si="5">CONCATENATE("('",E5,"', '",G5,"'),")</f>
+        <v>('first_name', 'First Name'),</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 301, CUSTOMER_FIELD_NAMES.age, "Age", _string)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <f t="shared" ref="I5:I50" si="6">SUBSTITUTE(A5,D5,CONCATENATE("CUSTOMER_FIELD_NAMES.",E5))</f>
+        <v xml:space="preserve">    _setup_field(_basic, 100, CUSTOMER_FIELD_NAMES.first_name, "First Name", _string)</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K50" si="7">CONCATENATE("def get_",E5,"(self):")</f>
+        <v>def get_first_name(self):</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>email", "Email", _string)</v>
+        <v>last_name", "Last Name", _string)</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
-        <v>email</v>
+        <v>last_name</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
-        <v>"email"</v>
+        <v>"last_name"</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>email</v>
+        <v>last_name</v>
       </c>
       <c r="F6" t="str">
         <f>RIGHT(B6, LEN(B6)-FIND("""",B6)-3)</f>
-        <v>Email", _string)</v>
+        <v>Last Name", _string)</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Email</v>
+        <v>Last Name</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="5"/>
-        <v>('email', 'Email'),</v>
+        <v>('last_name', 'Last Name'),</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 400, CUSTOMER_FIELD_NAMES.email, "Email", _string)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 200, CUSTOMER_FIELD_NAMES.last_name, "Last Name", _string)</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_last_name(self):</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>gender", "Gender", _string)</v>
+        <v>dob", "Birthday", _date)</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v>gender</v>
+        <v>dob</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
-        <v>"gender"</v>
+        <v>"dob"</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>gender</v>
+        <v>dob</v>
       </c>
       <c r="F7" t="str">
         <f>RIGHT(B7, LEN(B7)-FIND("""",B7)-3)</f>
-        <v>Gender", _string)</v>
+        <v>Birthday", _date)</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Gender</v>
+        <v>Birthday</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="5"/>
-        <v>('gender', 'Gender'),</v>
+        <v>('dob', 'Birthday'),</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 500, CUSTOMER_FIELD_NAMES.gender, "Gender", _string)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 300, CUSTOMER_FIELD_NAMES.dob, "Birthday", _date)</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_dob(self):</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>address#line1", "Address Line 1", _string)</v>
+        <v>age", "Age", _string)</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>address#line1</v>
+        <v>age</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
-        <v>"address#line1"</v>
+        <v>"age"</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>address__line1</v>
+        <v>age</v>
       </c>
       <c r="F8" t="str">
         <f>RIGHT(B8, LEN(B8)-FIND("""",B8)-3)</f>
-        <v>Address Line 1", _string)</v>
+        <v>Age", _string)</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Address Line 1</v>
+        <v>Age</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="5"/>
-        <v>('address__line1', 'Address Line 1'),</v>
+        <v>('age', 'Age'),</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 600, CUSTOMER_FIELD_NAMES.address__line1, "Address Line 1", _string)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 301, CUSTOMER_FIELD_NAMES.age, "Age", _string)</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_age(self):</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>address#line2", "Address Line 2", _string)</v>
+        <v>email", "Email", _string)</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>address#line2</v>
+        <v>email</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="2"/>
-        <v>"address#line2"</v>
+        <v>"email"</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>address__line2</v>
+        <v>email</v>
       </c>
       <c r="F9" t="str">
         <f>RIGHT(B9, LEN(B9)-FIND("""",B9)-3)</f>
-        <v>Address Line 2", _string)</v>
+        <v>Email", _string)</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Address Line 2</v>
+        <v>Email</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="5"/>
-        <v>('address__line2', 'Address Line 2'),</v>
+        <v>('email', 'Email'),</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 601, CUSTOMER_FIELD_NAMES.address__line2, "Address Line 2", _string)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 400, CUSTOMER_FIELD_NAMES.email, "Email", _string)</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_email(self):</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>address#city", "City", _string)</v>
+        <v>gender", "Gender", _string)</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>address#city</v>
+        <v>gender</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="2"/>
-        <v>"address#city"</v>
+        <v>"gender"</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>address__city</v>
+        <v>gender</v>
       </c>
       <c r="F10" t="str">
         <f>RIGHT(B10, LEN(B10)-FIND("""",B10)-3)</f>
-        <v>City", _string)</v>
+        <v>Gender", _string)</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>City</v>
+        <v>Gender</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="5"/>
-        <v>('address__city', 'City'),</v>
+        <v>('gender', 'Gender'),</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 700, CUSTOMER_FIELD_NAMES.address__city, "City", _string)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 500, CUSTOMER_FIELD_NAMES.gender, "Gender", _string)</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_gender(self):</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>address#zipcode", "ZipCode", _string)</v>
+        <v>address#line1", "Address Line 1", _string)</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>address#zipcode</v>
+        <v>address#line1</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="2"/>
-        <v>"address#zipcode"</v>
+        <v>"address#line1"</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>address__zipcode</v>
+        <v>address__line1</v>
       </c>
       <c r="F11" t="str">
         <f>RIGHT(B11, LEN(B11)-FIND("""",B11)-3)</f>
-        <v>ZipCode", _string)</v>
+        <v>Address Line 1", _string)</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>ZipCode</v>
+        <v>Address Line 1</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="5"/>
-        <v>('address__zipcode', 'ZipCode'),</v>
+        <v>('address__line1', 'Address Line 1'),</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 800, CUSTOMER_FIELD_NAMES.address__zipcode, "ZipCode", _string)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 600, CUSTOMER_FIELD_NAMES.address__line1, "Address Line 1", _string)</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_address__line1(self):</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>address#state", "State", _string)</v>
+        <v>address#line2", "Address Line 2", _string)</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>address#state</v>
+        <v>address#line2</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
-        <v>"address#state"</v>
+        <v>"address#line2"</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>address__state</v>
+        <v>address__line2</v>
       </c>
       <c r="F12" t="str">
         <f>RIGHT(B12, LEN(B12)-FIND("""",B12)-3)</f>
-        <v>State", _string)</v>
+        <v>Address Line 2", _string)</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>State</v>
+        <v>Address Line 2</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="5"/>
-        <v>('address__state', 'State'),</v>
+        <v>('address__line2', 'Address Line 2'),</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 900, CUSTOMER_FIELD_NAMES.address__state, "State", _string)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 601, CUSTOMER_FIELD_NAMES.address__line2, "Address Line 2", _string)</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_address__line2(self):</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>address#country", "Country", _string)</v>
+        <v>address#city", "City", _string)</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>address#country</v>
+        <v>address#city</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="2"/>
-        <v>"address#country"</v>
+        <v>"address#city"</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>address__country</v>
+        <v>address__city</v>
       </c>
       <c r="F13" t="str">
         <f>RIGHT(B13, LEN(B13)-FIND("""",B13)-3)</f>
-        <v>Country", _string)</v>
+        <v>City", _string)</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Country</v>
+        <v>City</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="5"/>
-        <v>('address__country', 'Country'),</v>
+        <v>('address__city', 'City'),</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 1000, CUSTOMER_FIELD_NAMES.address__country, "Country", _string)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 700, CUSTOMER_FIELD_NAMES.address__city, "City", _string)</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_address__city(self):</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>phone#mobile", "Mobile Phone", _string)</v>
+        <v>address#zipcode", "ZipCode", _string)</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>phone#mobile</v>
+        <v>address#zipcode</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="2"/>
-        <v>"phone#mobile"</v>
+        <v>"address#zipcode"</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>phone__mobile</v>
+        <v>address__zipcode</v>
       </c>
       <c r="F14" t="str">
         <f>RIGHT(B14, LEN(B14)-FIND("""",B14)-3)</f>
-        <v>Mobile Phone", _string)</v>
+        <v>ZipCode", _string)</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Mobile Phone</v>
+        <v>ZipCode</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="5"/>
-        <v>('phone__mobile', 'Mobile Phone'),</v>
+        <v>('address__zipcode', 'ZipCode'),</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 1100, CUSTOMER_FIELD_NAMES.phone__mobile, "Mobile Phone", _string)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 800, CUSTOMER_FIELD_NAMES.address__zipcode, "ZipCode", _string)</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_address__zipcode(self):</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>phone#home", "Home Phone", _string)</v>
+        <v>address#state", "State", _string)</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>phone#home</v>
+        <v>address#state</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="2"/>
-        <v>"phone#home"</v>
+        <v>"address#state"</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>phone__home</v>
+        <v>address__state</v>
       </c>
       <c r="F15" t="str">
         <f>RIGHT(B15, LEN(B15)-FIND("""",B15)-3)</f>
-        <v>Home Phone", _string)</v>
+        <v>State", _string)</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Home Phone</v>
+        <v>State</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="5"/>
-        <v>('phone__home', 'Home Phone'),</v>
+        <v>('address__state', 'State'),</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 1200, CUSTOMER_FIELD_NAMES.phone__home, "Home Phone", _string)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 900, CUSTOMER_FIELD_NAMES.address__state, "State", _string)</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_address__state(self):</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>occupation", "Occupation", _string)</v>
+        <v>address#country", "Country", _string)</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
-        <v>occupation</v>
+        <v>address#country</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="2"/>
-        <v>"occupation"</v>
+        <v>"address#country"</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>occupation</v>
+        <v>address__country</v>
       </c>
       <c r="F16" t="str">
         <f>RIGHT(B16, LEN(B16)-FIND("""",B16)-3)</f>
-        <v>Occupation", _string)</v>
+        <v>Country", _string)</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Occupation</v>
+        <v>Country</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="5"/>
-        <v>('occupation', 'Occupation'),</v>
+        <v>('address__country', 'Country'),</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 1300, CUSTOMER_FIELD_NAMES.occupation, "Occupation", _string)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 1000, CUSTOMER_FIELD_NAMES.address__country, "Country", _string)</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_address__country(self):</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>education", "Education", _string)</v>
+        <v>phone#mobile", "Mobile Phone", _string)</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
-        <v>education</v>
+        <v>phone#mobile</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="2"/>
-        <v>"education"</v>
+        <v>"phone#mobile"</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>education</v>
+        <v>phone__mobile</v>
       </c>
       <c r="F17" t="str">
         <f>RIGHT(B17, LEN(B17)-FIND("""",B17)-3)</f>
-        <v>Education", _string)</v>
+        <v>Mobile Phone", _string)</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Education</v>
+        <v>Mobile Phone</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="5"/>
-        <v>('education', 'Education'),</v>
+        <v>('phone__mobile', 'Mobile Phone'),</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_basic, 1400, CUSTOMER_FIELD_NAMES.education, "Education", _string)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 1100, CUSTOMER_FIELD_NAMES.phone__mobile, "Mobile Phone", _string)</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_phone__mobile(self):</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>marital_status", "Marital Status", _string)</v>
+        <v>phone#home", "Home Phone", _string)</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
-        <v>marital_status</v>
+        <v>phone#home</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="2"/>
-        <v>"marital_status"</v>
+        <v>"phone#home"</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>marital_status</v>
+        <v>phone__home</v>
       </c>
       <c r="F18" t="str">
         <f>RIGHT(B18, LEN(B18)-FIND("""",B18)-3)</f>
-        <v>Marital Status", _string)</v>
+        <v>Home Phone", _string)</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Marital Status</v>
+        <v>Home Phone</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="5"/>
-        <v>('marital_status', 'Marital Status'),</v>
+        <v>('phone__home', 'Home Phone'),</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 100, CUSTOMER_FIELD_NAMES.marital_status, "Marital Status", _string)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 1200, CUSTOMER_FIELD_NAMES.phone__home, "Home Phone", _string)</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_phone__home(self):</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>has_children", "Presence of Children", _bool)</v>
+        <v>occupation", "Occupation", _string)</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
-        <v>has_children</v>
+        <v>occupation</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="2"/>
-        <v>"has_children"</v>
+        <v>"occupation"</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>has_children</v>
+        <v>occupation</v>
       </c>
       <c r="F19" t="str">
         <f>RIGHT(B19, LEN(B19)-FIND("""",B19)-3)</f>
-        <v>Presence of Children", _bool)</v>
+        <v>Occupation", _string)</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Presence of Children</v>
+        <v>Occupation</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="5"/>
-        <v>('has_children', 'Presence of Children'),</v>
+        <v>('occupation', 'Occupation'),</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 200, CUSTOMER_FIELD_NAMES.has_children, "Presence of Children", _bool)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 1300, CUSTOMER_FIELD_NAMES.occupation, "Occupation", _string)</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_occupation(self):</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>home_owner_status", "Home Owner Status", _string)</v>
+        <v>education", "Education", _string)</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
-        <v>home_owner_status</v>
+        <v>education</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="2"/>
-        <v>"home_owner_status"</v>
+        <v>"education"</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>home_owner_status</v>
+        <v>education</v>
       </c>
       <c r="F20" t="str">
         <f>RIGHT(B20, LEN(B20)-FIND("""",B20)-3)</f>
-        <v>Home Owner Status", _string)</v>
+        <v>Education", _string)</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Home Owner Status</v>
+        <v>Education</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="5"/>
-        <v>('home_owner_status', 'Home Owner Status'),</v>
+        <v>('education', 'Education'),</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 300, CUSTOMER_FIELD_NAMES.home_owner_status, "Home Owner Status", _string)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_basic, 1400, CUSTOMER_FIELD_NAMES.education, "Education", _string)</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_education(self):</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>income", "Household Income", _string)</v>
+        <v>marital_status", "Marital Status", _string)</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
-        <v>income</v>
+        <v>marital_status</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="2"/>
-        <v>"income"</v>
+        <v>"marital_status"</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>income</v>
+        <v>marital_status</v>
       </c>
       <c r="F21" t="str">
         <f>RIGHT(B21, LEN(B21)-FIND("""",B21)-3)</f>
-        <v>Household Income", _string)</v>
+        <v>Marital Status", _string)</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Household Income</v>
+        <v>Marital Status</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="5"/>
-        <v>('income', 'Household Income'),</v>
+        <v>('marital_status', 'Marital Status'),</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 400, CUSTOMER_FIELD_NAMES.income, "Household Income", _string)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 100, CUSTOMER_FIELD_NAMES.marital_status, "Marital Status", _string)</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_marital_status(self):</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>home_market_value", "Home Market Value", _string)</v>
+        <v>has_children", "Presence of Children", _bool)</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
-        <v>home_market_value</v>
+        <v>has_children</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="2"/>
-        <v>"home_market_value"</v>
+        <v>"has_children"</v>
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>home_market_value</v>
+        <v>has_children</v>
       </c>
       <c r="F22" t="str">
         <f>RIGHT(B22, LEN(B22)-FIND("""",B22)-3)</f>
-        <v>Home Market Value", _string)</v>
+        <v>Presence of Children", _bool)</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Home Market Value</v>
+        <v>Presence of Children</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="5"/>
-        <v>('home_market_value', 'Home Market Value'),</v>
+        <v>('has_children', 'Presence of Children'),</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 500, CUSTOMER_FIELD_NAMES.home_market_value, "Home Market Value", _string)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 200, CUSTOMER_FIELD_NAMES.has_children, "Presence of Children", _bool)</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_has_children(self):</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>high_net_worth", "High Net Worth", _bool)</v>
+        <v>home_owner_status", "Home Owner Status", _string)</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
-        <v>high_net_worth</v>
+        <v>home_owner_status</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="2"/>
-        <v>"high_net_worth"</v>
+        <v>"home_owner_status"</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>high_net_worth</v>
+        <v>home_owner_status</v>
       </c>
       <c r="F23" t="str">
         <f>RIGHT(B23, LEN(B23)-FIND("""",B23)-3)</f>
-        <v>High Net Worth", _bool)</v>
+        <v>Home Owner Status", _string)</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>High Net Worth</v>
+        <v>Home Owner Status</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="5"/>
-        <v>('high_net_worth', 'High Net Worth'),</v>
+        <v>('home_owner_status', 'Home Owner Status'),</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 600, CUSTOMER_FIELD_NAMES.high_net_worth, "High Net Worth", _bool)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 300, CUSTOMER_FIELD_NAMES.home_owner_status, "Home Owner Status", _string)</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_home_owner_status(self):</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>length_of_residence", "Length of Residence",_bool)</v>
+        <v>income", "Household Income", _string)</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
-        <v>length_of_residence</v>
+        <v>income</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="2"/>
-        <v>"length_of_residence"</v>
+        <v>"income"</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>length_of_residence</v>
+        <v>income</v>
       </c>
       <c r="F24" t="str">
         <f>RIGHT(B24, LEN(B24)-FIND("""",B24)-3)</f>
-        <v>Length of Residence",_bool)</v>
+        <v>Household Income", _string)</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Length of Residence</v>
+        <v>Household Income</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="5"/>
-        <v>('length_of_residence', 'Length of Residence'),</v>
+        <v>('income', 'Household Income'),</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_household, 700, CUSTOMER_FIELD_NAMES.length_of_residence, "Length of Residence",_bool)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 400, CUSTOMER_FIELD_NAMES.income, "Household Income", _string)</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_income(self):</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>interest#arts", "Interest in Arts and Crafts", _bool)</v>
+        <v>home_market_value", "Home Market Value", _string)</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
-        <v>interest#arts</v>
+        <v>home_market_value</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="2"/>
-        <v>"interest#arts"</v>
+        <v>"home_market_value"</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>interest__arts</v>
+        <v>home_market_value</v>
       </c>
       <c r="F25" t="str">
         <f>RIGHT(B25, LEN(B25)-FIND("""",B25)-3)</f>
-        <v>Interest in Arts and Crafts", _bool)</v>
+        <v>Home Market Value", _string)</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Interest in Arts and Crafts</v>
+        <v>Home Market Value</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="5"/>
-        <v>('interest__arts', 'Interest in Arts and Crafts'),</v>
+        <v>('home_market_value', 'Home Market Value'),</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 100, CUSTOMER_FIELD_NAMES.interest__arts, "Interest in Arts and Crafts", _bool)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 500, CUSTOMER_FIELD_NAMES.home_market_value, "Home Market Value", _string)</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_home_market_value(self):</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>interest#blogging", "Interest in Blogging", _bool)</v>
+        <v>high_net_worth", "High Net Worth", _bool)</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
-        <v>interest#blogging</v>
+        <v>high_net_worth</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="2"/>
-        <v>"interest#blogging"</v>
+        <v>"high_net_worth"</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>interest__blogging</v>
+        <v>high_net_worth</v>
       </c>
       <c r="F26" t="str">
         <f>RIGHT(B26, LEN(B26)-FIND("""",B26)-3)</f>
-        <v>Interest in Blogging", _bool)</v>
+        <v>High Net Worth", _bool)</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Interest in Blogging</v>
+        <v>High Net Worth</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="5"/>
-        <v>('interest__blogging', 'Interest in Blogging'),</v>
+        <v>('high_net_worth', 'High Net Worth'),</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 200, CUSTOMER_FIELD_NAMES.interest__blogging, "Interest in Blogging", _bool)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 600, CUSTOMER_FIELD_NAMES.high_net_worth, "High Net Worth", _bool)</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_high_net_worth(self):</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>interest#books", "Interest in Books", _bool)</v>
+        <v>length_of_residence", "Length of Residence",_bool)</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
-        <v>interest#books</v>
+        <v>length_of_residence</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="2"/>
-        <v>"interest#books"</v>
+        <v>"length_of_residence"</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>interest__books</v>
+        <v>length_of_residence</v>
       </c>
       <c r="F27" t="str">
         <f>RIGHT(B27, LEN(B27)-FIND("""",B27)-3)</f>
-        <v>Interest in Books", _bool)</v>
+        <v>Length of Residence",_bool)</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Interest in Books</v>
+        <v>Length of Residence</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="5"/>
-        <v>('interest__books', 'Interest in Books'),</v>
+        <v>('length_of_residence', 'Length of Residence'),</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 300, CUSTOMER_FIELD_NAMES.interest__books, "Interest in Books", _bool)</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_household, 700, CUSTOMER_FIELD_NAMES.length_of_residence, "Length of Residence",_bool)</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_length_of_residence(self):</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>interest#business", "Interest in Business", _bool)</v>
+        <v>interest#arts", "Interest in Arts and Crafts", _bool)</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
-        <v>interest#business</v>
+        <v>interest#arts</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="2"/>
-        <v>"interest#business"</v>
+        <v>"interest#arts"</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>interest__business</v>
+        <v>interest__arts</v>
       </c>
       <c r="F28" t="str">
         <f>RIGHT(B28, LEN(B28)-FIND("""",B28)-3)</f>
-        <v>Interest in Business", _bool)</v>
+        <v>Interest in Arts and Crafts", _bool)</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Interest in Business</v>
+        <v>Interest in Arts and Crafts</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="5"/>
-        <v>('interest__business', 'Interest in Business'),</v>
+        <v>('interest__arts', 'Interest in Arts and Crafts'),</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 400, CUSTOMER_FIELD_NAMES.interest__business, "Interest in Business", _bool)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 100, CUSTOMER_FIELD_NAMES.interest__arts, "Interest in Arts and Crafts", _bool)</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_interest__arts(self):</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>interest#health", "Interest in Health and Wellness", _bool)</v>
+        <v>interest#blogging", "Interest in Blogging", _bool)</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
-        <v>interest#health</v>
+        <v>interest#blogging</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="2"/>
-        <v>"interest#health"</v>
+        <v>"interest#blogging"</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>interest__health</v>
+        <v>interest__blogging</v>
       </c>
       <c r="F29" t="str">
         <f>RIGHT(B29, LEN(B29)-FIND("""",B29)-3)</f>
-        <v>Interest in Health and Wellness", _bool)</v>
+        <v>Interest in Blogging", _bool)</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Interest in Health and Wellness</v>
+        <v>Interest in Blogging</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="5"/>
-        <v>('interest__health', 'Interest in Health and Wellness'),</v>
+        <v>('interest__blogging', 'Interest in Blogging'),</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 500, CUSTOMER_FIELD_NAMES.interest__health, "Interest in Health and Wellness", _bool)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 200, CUSTOMER_FIELD_NAMES.interest__blogging, "Interest in Blogging", _bool)</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_interest__blogging(self):</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>interest#news", "Interest in News and Current Events", _bool)</v>
+        <v>interest#books", "Interest in Books", _bool)</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
-        <v>interest#news</v>
+        <v>interest#books</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="2"/>
-        <v>"interest#news"</v>
+        <v>"interest#books"</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>interest__news</v>
+        <v>interest__books</v>
       </c>
       <c r="F30" t="str">
         <f>RIGHT(B30, LEN(B30)-FIND("""",B30)-3)</f>
-        <v>Interest in News and Current Events", _bool)</v>
+        <v>Interest in Books", _bool)</v>
       </c>
       <c r="G30" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Interest in News and Current Events</v>
+        <v>Interest in Books</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="5"/>
-        <v>('interest__news', 'Interest in News and Current Events'),</v>
+        <v>('interest__books', 'Interest in Books'),</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 600, CUSTOMER_FIELD_NAMES.interest__news, "Interest in News and Current Events", _bool)</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 300, CUSTOMER_FIELD_NAMES.interest__books, "Interest in Books", _bool)</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_interest__books(self):</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#automotive", "Purchases Automotive Goods", _bool)</v>
+        <v>interest#business", "Interest in Business", _bool)</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#automotive</v>
+        <v>interest#business</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#automotive"</v>
+        <v>"interest#business"</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__automotive</v>
+        <v>interest__business</v>
       </c>
       <c r="F31" t="str">
         <f>RIGHT(B31, LEN(B31)-FIND("""",B31)-3)</f>
-        <v>Purchases Automotive Goods", _bool)</v>
+        <v>Interest in Business", _bool)</v>
       </c>
       <c r="G31" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Automotive Goods</v>
+        <v>Interest in Business</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__automotive', 'Purchases Automotive Goods'),</v>
+        <v>('interest__business', 'Interest in Business'),</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 100, CUSTOMER_FIELD_NAMES.purchase__automotive, "Purchases Automotive Goods", _bool)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 400, CUSTOMER_FIELD_NAMES.interest__business, "Interest in Business", _bool)</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_interest__business(self):</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#baby", "Has Bought a Baby Product", _bool)</v>
+        <v>interest#health", "Interest in Health and Wellness", _bool)</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#baby</v>
+        <v>interest#health</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#baby"</v>
+        <v>"interest#health"</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__baby</v>
+        <v>interest__health</v>
       </c>
       <c r="F32" t="str">
         <f>RIGHT(B32, LEN(B32)-FIND("""",B32)-3)</f>
-        <v>Has Bought a Baby Product", _bool)</v>
+        <v>Interest in Health and Wellness", _bool)</v>
       </c>
       <c r="G32" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Has Bought a Baby Product</v>
+        <v>Interest in Health and Wellness</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__baby', 'Has Bought a Baby Product'),</v>
+        <v>('interest__health', 'Interest in Health and Wellness'),</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 200, CUSTOMER_FIELD_NAMES.purchase__baby, "Has Bought a Baby Product", _bool)</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 500, CUSTOMER_FIELD_NAMES.interest__health, "Interest in Health and Wellness", _bool)</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_interest__health(self):</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#beauty", "Purchases Beauty Products", _bool)</v>
+        <v>interest#news", "Interest in News and Current Events", _bool)</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#beauty</v>
+        <v>interest#news</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#beauty"</v>
+        <v>"interest#news"</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__beauty</v>
+        <v>interest__news</v>
       </c>
       <c r="F33" t="str">
         <f>RIGHT(B33, LEN(B33)-FIND("""",B33)-3)</f>
-        <v>Purchases Beauty Products", _bool)</v>
+        <v>Interest in News and Current Events", _bool)</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Beauty Products</v>
+        <v>Interest in News and Current Events</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__beauty', 'Purchases Beauty Products'),</v>
+        <v>('interest__news', 'Interest in News and Current Events'),</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 300, CUSTOMER_FIELD_NAMES.purchase__beauty, "Purchases Beauty Products", _bool)</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 600, CUSTOMER_FIELD_NAMES.interest__news, "Interest in News and Current Events", _bool)</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_interest__news(self):</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#charitable","Indicates liklihood of Being a Charitable Donor", _bool)</v>
+        <v>purchase#automotive", "Purchases Automotive Goods", _bool)</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#charitable</v>
+        <v>purchase#automotive</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#charitable"</v>
+        <v>"purchase#automotive"</v>
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__charitable</v>
-      </c>
-      <c r="F34" t="s">
-        <v>47</v>
+        <v>purchase__automotive</v>
+      </c>
+      <c r="F34" t="str">
+        <f>RIGHT(B34, LEN(B34)-FIND("""",B34)-3)</f>
+        <v>Purchases Automotive Goods", _bool)</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Indicates liklihood of Being a Charitable Donor</v>
+        <v>Purchases Automotive Goods</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__charitable', 'Indicates liklihood of Being a Charitable Donor'),</v>
+        <v>('purchase__automotive', 'Purchases Automotive Goods'),</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 400, CUSTOMER_FIELD_NAMES.purchase__charitable,"Indicates liklihood of Being a Charitable Donor", _bool)</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 100, CUSTOMER_FIELD_NAMES.purchase__automotive, "Purchases Automotive Goods", _bool)</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__automotive(self):</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#cooking", "Purchases cooking magazines; interest in cooking", _bool)</v>
+        <v>purchase#baby", "Has Bought a Baby Product", _bool)</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#cooking</v>
+        <v>purchase#baby</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#cooking"</v>
+        <v>"purchase#baby"</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__cooking</v>
+        <v>purchase__baby</v>
       </c>
       <c r="F35" t="str">
         <f>RIGHT(B35, LEN(B35)-FIND("""",B35)-3)</f>
-        <v>Purchases cooking magazines; interest in cooking", _bool)</v>
+        <v>Has Bought a Baby Product", _bool)</v>
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases cooking magazines; interest in cooking</v>
+        <v>Has Bought a Baby Product</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__cooking', 'Purchases cooking magazines; interest in cooking'),</v>
+        <v>('purchase__baby', 'Has Bought a Baby Product'),</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 500, CUSTOMER_FIELD_NAMES.purchase__cooking, "Purchases cooking magazines; interest in cooking", _bool)</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 200, CUSTOMER_FIELD_NAMES.purchase__baby, "Has Bought a Baby Product", _bool)</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__baby(self):</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#discount", "Purchase behavior: Interest in discounts", _bool)</v>
+        <v>purchase#beauty", "Purchases Beauty Products", _bool)</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#discount</v>
+        <v>purchase#beauty</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#discount"</v>
+        <v>"purchase#beauty"</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__discount</v>
+        <v>purchase__beauty</v>
       </c>
       <c r="F36" t="str">
         <f>RIGHT(B36, LEN(B36)-FIND("""",B36)-3)</f>
-        <v>Purchase behavior: Interest in discounts", _bool)</v>
+        <v>Purchases Beauty Products", _bool)</v>
       </c>
       <c r="G36" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchase behavior: Interest in discounts</v>
+        <v>Purchases Beauty Products</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__discount', 'Purchase behavior: Interest in discounts'),</v>
+        <v>('purchase__beauty', 'Purchases Beauty Products'),</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 600, CUSTOMER_FIELD_NAMES.purchase__discount, "Purchase behavior: Interest in discounts", _bool)</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 300, CUSTOMER_FIELD_NAMES.purchase__beauty, "Purchases Beauty Products", _bool)</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__beauty(self):</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#high_end_brands", "Has bought a premium CPG brand in the past 18 months ", _bool)</v>
+        <v>purchase#charitable","Indicates liklihood of Being a Charitable Donor", _bool)</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#high_end_brands</v>
+        <v>purchase#charitable</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#high_end_brands"</v>
+        <v>"purchase#charitable"</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__high_end_brands</v>
-      </c>
-      <c r="F37" t="str">
-        <f>RIGHT(B37, LEN(B37)-FIND("""",B37)-3)</f>
-        <v>Has bought a premium CPG brand in the past 18 months ", _bool)</v>
+        <v>purchase__charitable</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
       </c>
       <c r="G37" s="2" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">Has bought a premium CPG brand in the past 18 months </v>
+        <v>Indicates liklihood of Being a Charitable Donor</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__high_end_brands', 'Has bought a premium CPG brand in the past 18 months '),</v>
+        <v>('purchase__charitable', 'Indicates liklihood of Being a Charitable Donor'),</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 700, CUSTOMER_FIELD_NAMES.purchase__high_end_brands, "Has bought a premium CPG brand in the past 18 months ", _bool)</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 400, CUSTOMER_FIELD_NAMES.purchase__charitable,"Indicates liklihood of Being a Charitable Donor", _bool)</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__charitable(self):</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#home_garden", "Purchases Home &amp; Garden Products", _bool)</v>
+        <v>purchase#cooking", "Purchases cooking magazines; interest in cooking", _bool)</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#home_garden</v>
+        <v>purchase#cooking</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#home_garden"</v>
+        <v>"purchase#cooking"</v>
       </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__home_garden</v>
+        <v>purchase__cooking</v>
       </c>
       <c r="F38" t="str">
         <f>RIGHT(B38, LEN(B38)-FIND("""",B38)-3)</f>
-        <v>Purchases Home &amp; Garden Products", _bool)</v>
+        <v>Purchases cooking magazines; interest in cooking", _bool)</v>
       </c>
       <c r="G38" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Home &amp; Garden Products</v>
+        <v>Purchases cooking magazines; interest in cooking</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__home_garden', 'Purchases Home &amp; Garden Products'),</v>
+        <v>('purchase__cooking', 'Purchases cooking magazines; interest in cooking'),</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 800, CUSTOMER_FIELD_NAMES.purchase__home_garden, "Purchases Home &amp; Garden Products", _bool)</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 500, CUSTOMER_FIELD_NAMES.purchase__cooking, "Purchases cooking magazines; interest in cooking", _bool)</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__cooking(self):</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#home_improvement", "Purchases Home Improvement Products", _bool)</v>
+        <v>purchase#discount", "Purchase behavior: Interest in discounts", _bool)</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#home_improvement</v>
+        <v>purchase#discount</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#home_improvement"</v>
+        <v>"purchase#discount"</v>
       </c>
       <c r="E39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__home_improvement</v>
+        <v>purchase__discount</v>
       </c>
       <c r="F39" t="str">
         <f>RIGHT(B39, LEN(B39)-FIND("""",B39)-3)</f>
-        <v>Purchases Home Improvement Products", _bool)</v>
+        <v>Purchase behavior: Interest in discounts", _bool)</v>
       </c>
       <c r="G39" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Home Improvement Products</v>
+        <v>Purchase behavior: Interest in discounts</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__home_improvement', 'Purchases Home Improvement Products'),</v>
+        <v>('purchase__discount', 'Purchase behavior: Interest in discounts'),</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 900, CUSTOMER_FIELD_NAMES.purchase__home_improvement, "Purchases Home Improvement Products", _bool)</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 600, CUSTOMER_FIELD_NAMES.purchase__discount, "Purchase behavior: Interest in discounts", _bool)</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__discount(self):</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#luxury", "Purchases Luxury Items", _bool)</v>
+        <v>purchase#high_end_brands", "Has bought a premium CPG brand in the past 18 months ", _bool)</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#luxury</v>
+        <v>purchase#high_end_brands</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#luxury"</v>
+        <v>"purchase#high_end_brands"</v>
       </c>
       <c r="E40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__luxury</v>
+        <v>purchase__high_end_brands</v>
       </c>
       <c r="F40" t="str">
         <f>RIGHT(B40, LEN(B40)-FIND("""",B40)-3)</f>
-        <v>Purchases Luxury Items", _bool)</v>
+        <v>Has bought a premium CPG brand in the past 18 months ", _bool)</v>
       </c>
       <c r="G40" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Luxury Items</v>
+        <v xml:space="preserve">Has bought a premium CPG brand in the past 18 months </v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__luxury', 'Purchases Luxury Items'),</v>
+        <v>('purchase__high_end_brands', 'Has bought a premium CPG brand in the past 18 months '),</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1000, CUSTOMER_FIELD_NAMES.purchase__luxury, "Purchases Luxury Items", _bool)</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 700, CUSTOMER_FIELD_NAMES.purchase__high_end_brands, "Has bought a premium CPG brand in the past 18 months ", _bool)</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__high_end_brands(self):</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#magazine", "Purchases Magazine Subscriptions", _bool)</v>
+        <v>purchase#home_garden", "Purchases Home &amp; Garden Products", _bool)</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#magazine</v>
+        <v>purchase#home_garden</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#magazine"</v>
+        <v>"purchase#home_garden"</v>
       </c>
       <c r="E41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__magazine</v>
+        <v>purchase__home_garden</v>
       </c>
       <c r="F41" t="str">
         <f>RIGHT(B41, LEN(B41)-FIND("""",B41)-3)</f>
-        <v>Purchases Magazine Subscriptions", _bool)</v>
+        <v>Purchases Home &amp; Garden Products", _bool)</v>
       </c>
       <c r="G41" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Magazine Subscriptions</v>
+        <v>Purchases Home &amp; Garden Products</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__magazine', 'Purchases Magazine Subscriptions'),</v>
+        <v>('purchase__home_garden', 'Purchases Home &amp; Garden Products'),</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1100, CUSTOMER_FIELD_NAMES.purchase__magazine, "Purchases Magazine Subscriptions", _bool)</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 800, CUSTOMER_FIELD_NAMES.purchase__home_garden, "Purchases Home &amp; Garden Products", _bool)</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__home_garden(self):</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#outdoor", "Purchases Outdoor and Adventure Products", _bool)</v>
+        <v>purchase#home_improvement", "Purchases Home Improvement Products", _bool)</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#outdoor</v>
+        <v>purchase#home_improvement</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#outdoor"</v>
+        <v>"purchase#home_improvement"</v>
       </c>
       <c r="E42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__outdoor</v>
+        <v>purchase__home_improvement</v>
       </c>
       <c r="F42" t="str">
         <f>RIGHT(B42, LEN(B42)-FIND("""",B42)-3)</f>
-        <v>Purchases Outdoor and Adventure Products", _bool)</v>
+        <v>Purchases Home Improvement Products", _bool)</v>
       </c>
       <c r="G42" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Outdoor and Adventure Products</v>
+        <v>Purchases Home Improvement Products</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__outdoor', 'Purchases Outdoor and Adventure Products'),</v>
+        <v>('purchase__home_improvement', 'Purchases Home Improvement Products'),</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1200, CUSTOMER_FIELD_NAMES.purchase__outdoor, "Purchases Outdoor and Adventure Products", _bool)</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 900, CUSTOMER_FIELD_NAMES.purchase__home_improvement, "Purchases Home Improvement Products", _bool)</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__home_improvement(self):</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#pets", "Purchases Pet Related Products", _bool)</v>
+        <v>purchase#luxury", "Purchases Luxury Items", _bool)</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#pets</v>
+        <v>purchase#luxury</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#pets"</v>
+        <v>"purchase#luxury"</v>
       </c>
       <c r="E43" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__pets</v>
+        <v>purchase__luxury</v>
       </c>
       <c r="F43" t="str">
         <f>RIGHT(B43, LEN(B43)-FIND("""",B43)-3)</f>
-        <v>Purchases Pet Related Products", _bool)</v>
+        <v>Purchases Luxury Items", _bool)</v>
       </c>
       <c r="G43" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Pet Related Products</v>
+        <v>Purchases Luxury Items</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__pets', 'Purchases Pet Related Products'),</v>
+        <v>('purchase__luxury', 'Purchases Luxury Items'),</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1300, CUSTOMER_FIELD_NAMES.purchase__pets, "Purchases Pet Related Products", _bool)</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 1000, CUSTOMER_FIELD_NAMES.purchase__luxury, "Purchases Luxury Items", _bool)</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__luxury(self):</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#power_shopper", "Purchases Items from Multiple Retail Channels", _bool)</v>
+        <v>purchase#magazine", "Purchases Magazine Subscriptions", _bool)</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#power_shopper</v>
+        <v>purchase#magazine</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#power_shopper"</v>
+        <v>"purchase#magazine"</v>
       </c>
       <c r="E44" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__power_shopper</v>
+        <v>purchase__magazine</v>
       </c>
       <c r="F44" t="str">
         <f>RIGHT(B44, LEN(B44)-FIND("""",B44)-3)</f>
-        <v>Purchases Items from Multiple Retail Channels", _bool)</v>
+        <v>Purchases Magazine Subscriptions", _bool)</v>
       </c>
       <c r="G44" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Items from Multiple Retail Channels</v>
+        <v>Purchases Magazine Subscriptions</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__power_shopper', 'Purchases Items from Multiple Retail Channels'),</v>
+        <v>('purchase__magazine', 'Purchases Magazine Subscriptions'),</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1400, CUSTOMER_FIELD_NAMES.purchase__power_shopper, "Purchases Items from Multiple Retail Channels", _bool)</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 1100, CUSTOMER_FIELD_NAMES.purchase__magazine, "Purchases Magazine Subscriptions", _bool)</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__magazine(self):</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#sports", "Purchases Sporting Goods / Sports Related Products", _bool)</v>
+        <v>purchase#outdoor", "Purchases Outdoor and Adventure Products", _bool)</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#sports</v>
+        <v>purchase#outdoor</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#sports"</v>
+        <v>"purchase#outdoor"</v>
       </c>
       <c r="E45" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__sports</v>
+        <v>purchase__outdoor</v>
       </c>
       <c r="F45" t="str">
         <f>RIGHT(B45, LEN(B45)-FIND("""",B45)-3)</f>
-        <v>Purchases Sporting Goods / Sports Related Products", _bool)</v>
+        <v>Purchases Outdoor and Adventure Products", _bool)</v>
       </c>
       <c r="G45" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Sporting Goods / Sports Related Products</v>
+        <v>Purchases Outdoor and Adventure Products</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__sports', 'Purchases Sporting Goods / Sports Related Products'),</v>
+        <v>('purchase__outdoor', 'Purchases Outdoor and Adventure Products'),</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1500, CUSTOMER_FIELD_NAMES.purchase__sports, "Purchases Sporting Goods / Sports Related Products", _bool)</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 1200, CUSTOMER_FIELD_NAMES.purchase__outdoor, "Purchases Outdoor and Adventure Products", _bool)</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__outdoor(self):</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#technology", "Purchases Technology Products", _bool)</v>
+        <v>purchase#pets", "Purchases Pet Related Products", _bool)</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#technology</v>
+        <v>purchase#pets</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#technology"</v>
+        <v>"purchase#pets"</v>
       </c>
       <c r="E46" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__technology</v>
+        <v>purchase__pets</v>
       </c>
       <c r="F46" t="str">
         <f>RIGHT(B46, LEN(B46)-FIND("""",B46)-3)</f>
-        <v>Purchases Technology Products", _bool)</v>
+        <v>Purchases Pet Related Products", _bool)</v>
       </c>
       <c r="G46" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>Purchases Technology Products</v>
+        <v>Purchases Pet Related Products</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="5"/>
-        <v>('purchase__technology', 'Purchases Technology Products'),</v>
+        <v>('purchase__pets', 'Purchases Pet Related Products'),</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">    _setup_field(_custom, 1600, CUSTOMER_FIELD_NAMES.purchase__technology, "Purchases Technology Products", _bool)</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v xml:space="preserve">    _setup_field(_custom, 1300, CUSTOMER_FIELD_NAMES.purchase__pets, "Purchases Pet Related Products", _bool)</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__pets(self):</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>purchase#travel", "Purchases Travel Related Goods", _bool)</v>
+        <v>purchase#power_shopper", "Purchases Items from Multiple Retail Channels", _bool)</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
-        <v>purchase#travel</v>
+        <v>purchase#power_shopper</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="2"/>
-        <v>"purchase#travel"</v>
+        <v>"purchase#power_shopper"</v>
       </c>
       <c r="E47" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>purchase__travel</v>
+        <v>purchase__power_shopper</v>
       </c>
       <c r="F47" t="str">
         <f>RIGHT(B47, LEN(B47)-FIND("""",B47)-3)</f>
+        <v>Purchases Items from Multiple Retail Channels", _bool)</v>
+      </c>
+      <c r="G47" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Purchases Items from Multiple Retail Channels</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="5"/>
+        <v>('purchase__power_shopper', 'Purchases Items from Multiple Retail Channels'),</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    _setup_field(_custom, 1400, CUSTOMER_FIELD_NAMES.purchase__power_shopper, "Purchases Items from Multiple Retail Channels", _bool)</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__power_shopper(self):</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>purchase#sports", "Purchases Sporting Goods / Sports Related Products", _bool)</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="1"/>
+        <v>purchase#sports</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>"purchase#sports"</v>
+      </c>
+      <c r="E48" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>purchase__sports</v>
+      </c>
+      <c r="F48" t="str">
+        <f>RIGHT(B48, LEN(B48)-FIND("""",B48)-3)</f>
+        <v>Purchases Sporting Goods / Sports Related Products", _bool)</v>
+      </c>
+      <c r="G48" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Purchases Sporting Goods / Sports Related Products</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="5"/>
+        <v>('purchase__sports', 'Purchases Sporting Goods / Sports Related Products'),</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    _setup_field(_custom, 1500, CUSTOMER_FIELD_NAMES.purchase__sports, "Purchases Sporting Goods / Sports Related Products", _bool)</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__sports(self):</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>purchase#technology", "Purchases Technology Products", _bool)</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="1"/>
+        <v>purchase#technology</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>"purchase#technology"</v>
+      </c>
+      <c r="E49" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>purchase__technology</v>
+      </c>
+      <c r="F49" t="str">
+        <f>RIGHT(B49, LEN(B49)-FIND("""",B49)-3)</f>
+        <v>Purchases Technology Products", _bool)</v>
+      </c>
+      <c r="G49" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>Purchases Technology Products</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="5"/>
+        <v>('purchase__technology', 'Purchases Technology Products'),</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    _setup_field(_custom, 1600, CUSTOMER_FIELD_NAMES.purchase__technology, "Purchases Technology Products", _bool)</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__technology(self):</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>purchase#travel", "Purchases Travel Related Goods", _bool)</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="1"/>
+        <v>purchase#travel</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>"purchase#travel"</v>
+      </c>
+      <c r="E50" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>purchase__travel</v>
+      </c>
+      <c r="F50" t="str">
+        <f>RIGHT(B50, LEN(B50)-FIND("""",B50)-3)</f>
         <v>Purchases Travel Related Goods", _bool)</v>
       </c>
-      <c r="G47" s="2" t="str">
+      <c r="G50" s="2" t="str">
         <f t="shared" si="4"/>
         <v>Purchases Travel Related Goods</v>
       </c>
-      <c r="H47" t="str">
+      <c r="H50" t="str">
         <f t="shared" si="5"/>
         <v>('purchase__travel', 'Purchases Travel Related Goods'),</v>
       </c>
-      <c r="I47" t="str">
+      <c r="I50" t="str">
         <f t="shared" si="6"/>
         <v xml:space="preserve">    _setup_field(_custom, 1700, CUSTOMER_FIELD_NAMES.purchase__travel, "Purchases Travel Related Goods", _bool)</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="7"/>
+        <v>def get_purchase__travel(self):</v>
       </c>
     </row>
   </sheetData>

</xml_diff>